<commit_message>
commit before going home
</commit_message>
<xml_diff>
--- a/RoutingPlan.xlsx
+++ b/RoutingPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
   <si>
     <t>no</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>post addUser as admin</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>routers</t>
+  </si>
+  <si>
+    <t>ejs page</t>
   </si>
 </sst>
 </file>
@@ -223,11 +232,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E26"/>
+  <dimension ref="B3:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +532,7 @@
     <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,8 +545,14 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -549,8 +565,11 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -564,7 +583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -578,7 +597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -592,7 +611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -606,7 +625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -619,8 +638,11 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -634,7 +656,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -648,7 +670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>9</v>
       </c>
@@ -662,7 +684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -676,7 +698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>11</v>
       </c>
@@ -690,7 +712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>12</v>
       </c>
@@ -704,7 +726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
test upload to github
</commit_message>
<xml_diff>
--- a/RoutingPlan.xlsx
+++ b/RoutingPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
   <si>
     <t>no</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>ejs page</t>
+  </si>
+  <si>
+    <t>NANTI</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>XXX</t>
   </si>
 </sst>
 </file>
@@ -518,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G26"/>
+  <dimension ref="B3:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +538,7 @@
     <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -582,6 +591,9 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
@@ -596,6 +608,9 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -609,6 +624,9 @@
       </c>
       <c r="E7" t="s">
         <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -624,260 +642,317 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="3">
-        <v>14</v>
-      </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
         <v>42</v>
       </c>
       <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="3">
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
-        <v>16</v>
-      </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
       </c>
       <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="3">
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
         <v>17</v>
       </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>29</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
         <v>18</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>31</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
         <v>20</v>
       </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>35</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>37</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
         <v>22</v>
       </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
         <v>39</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
         <v>23</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" t="s">
         <v>39</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>41</v>
+      </c>
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push before break, login and register page done
</commit_message>
<xml_diff>
--- a/RoutingPlan.xlsx
+++ b/RoutingPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>no</t>
   </si>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,6 +577,9 @@
       <c r="F4" t="s">
         <v>45</v>
       </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
@@ -594,6 +597,9 @@
       <c r="F5" t="s">
         <v>45</v>
       </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
@@ -611,6 +617,9 @@
       <c r="F6" t="s">
         <v>45</v>
       </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -626,6 +635,9 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -643,6 +655,9 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
eve commit, logins/logout done, user profile, enroll, mycourse done, lack courseDetail
</commit_message>
<xml_diff>
--- a/RoutingPlan.xlsx
+++ b/RoutingPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Radityo Prakoso\Hacktiv8\phase_1\week4\Day3\pair project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Radityo Prakoso\Hacktiv8\phase_1\week4\Day3\pp New\pairproject-p1-hck65-edu-koso-rizki\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
   <si>
     <t>no</t>
   </si>
@@ -161,9 +161,6 @@
     <t>post addUser as admin</t>
   </si>
   <si>
-    <t>v</t>
-  </si>
-  <si>
     <t>routers</t>
   </si>
   <si>
@@ -177,6 +174,12 @@
   </si>
   <si>
     <t>XXX</t>
+  </si>
+  <si>
+    <t>VV</t>
+  </si>
+  <si>
+    <t>PDFJS-DIST</t>
   </si>
 </sst>
 </file>
@@ -529,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,10 +558,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -575,10 +578,10 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -595,10 +598,10 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -615,10 +618,10 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -635,10 +638,10 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -655,10 +658,10 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -678,7 +681,7 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -695,7 +698,7 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -712,7 +715,7 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -729,7 +732,7 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -746,7 +749,7 @@
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -763,7 +766,7 @@
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -780,7 +783,7 @@
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -831,10 +834,10 @@
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -851,10 +854,10 @@
         <v>28</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -873,6 +876,12 @@
       <c r="E22" t="s">
         <v>30</v>
       </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
@@ -887,6 +896,12 @@
       <c r="E23" t="s">
         <v>32</v>
       </c>
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
@@ -901,6 +916,12 @@
       <c r="E24" t="s">
         <v>34</v>
       </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
@@ -915,6 +936,9 @@
       <c r="E25" t="s">
         <v>36</v>
       </c>
+      <c r="H25" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
@@ -929,6 +953,12 @@
       <c r="E26" t="s">
         <v>38</v>
       </c>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
@@ -944,10 +974,10 @@
         <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -964,10 +994,10 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PP lack mvp feature only
</commit_message>
<xml_diff>
--- a/RoutingPlan.xlsx
+++ b/RoutingPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
   <si>
     <t>no</t>
   </si>
@@ -170,9 +170,6 @@
     <t>NANTI</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>XXX</t>
   </si>
   <si>
@@ -180,6 +177,27 @@
   </si>
   <si>
     <t>PDFJS-DIST</t>
+  </si>
+  <si>
+    <t>rev</t>
+  </si>
+  <si>
+    <t>link type dkit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rev </t>
+  </si>
+  <si>
+    <t>tabel udah jadi</t>
+  </si>
+  <si>
+    <t>fungsi selesai</t>
+  </si>
+  <si>
+    <t>SEARCHBAR</t>
+  </si>
+  <si>
+    <t>BLOM DIO</t>
   </si>
 </sst>
 </file>
@@ -530,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H28"/>
+  <dimension ref="B3:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,9 +560,11 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -564,7 +584,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -578,13 +598,13 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -598,13 +618,13 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -618,13 +638,13 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -638,13 +658,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -658,16 +678,16 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>6</v>
       </c>
@@ -681,10 +701,16 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>7</v>
       </c>
@@ -698,10 +724,19 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>8</v>
       </c>
@@ -715,10 +750,16 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>9</v>
       </c>
@@ -732,10 +773,16 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>10</v>
       </c>
@@ -749,10 +796,16 @@
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>11</v>
       </c>
@@ -766,10 +819,16 @@
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>12</v>
       </c>
@@ -783,7 +842,13 @@
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -800,7 +865,7 @@
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -817,7 +882,7 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -834,7 +899,7 @@
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H19" t="s">
         <v>47</v>
@@ -854,7 +919,7 @@
         <v>28</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" t="s">
         <v>47</v>
@@ -877,10 +942,10 @@
         <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -897,10 +962,10 @@
         <v>32</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -917,10 +982,10 @@
         <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -937,7 +1002,7 @@
         <v>36</v>
       </c>
       <c r="H25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -954,10 +1019,10 @@
         <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -974,7 +1039,7 @@
         <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
         <v>47</v>
@@ -994,10 +1059,18 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H28" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>56</v>
+      </c>
+      <c r="H29" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>